<commit_message>
Deaths from 2004 to 2014 Planilha Excel
</commit_message>
<xml_diff>
--- a/fiocruz/deaths_2004_2014/TotalObitosPorAnoEstado2004-2014.xlsx
+++ b/fiocruz/deaths_2004_2014/TotalObitosPorAnoEstado2004-2014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="TotalObitosPorAnoEstado2004-201" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,6 @@
     <sheet name="Óbitos Categoria CID-10" sheetId="7" r:id="rId6"/>
     <sheet name="Mortes sem Assistência" sheetId="8" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
@@ -3815,6 +3812,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Óbitos até 1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> ano entre 2004 a 2014</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -4203,7 +4230,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5375,7 +5401,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5487,7 +5512,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5686,9 +5710,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-5F4C-4A29-A53F-0C001BACB83F}"/>
                 </c:ext>
@@ -5710,9 +5732,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-5F4C-4A29-A53F-0C001BACB83F}"/>
                 </c:ext>
@@ -5785,9 +5805,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5871,7 +5889,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -5999,7 +6016,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6611,7 +6627,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6798,6 +6813,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-A44E-4CB5-8C0B-DD392F7D49C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -6817,6 +6837,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-A44E-4CB5-8C0B-DD392F7D49C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -6836,6 +6861,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-A44E-4CB5-8C0B-DD392F7D49C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -6855,6 +6885,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-A44E-4CB5-8C0B-DD392F7D49C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -6874,6 +6909,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-A44E-4CB5-8C0B-DD392F7D49C7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
@@ -7181,7 +7221,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11234,444 +11273,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Óbitos por UF Residência (49)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Menos 22 semanas</v>
-          </cell>
-          <cell r="C10">
-            <v>15431</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>2</v>
-          </cell>
-          <cell r="C11">
-            <v>7472</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>2</v>
-          </cell>
-          <cell r="C12">
-            <v>7584</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>2</v>
-          </cell>
-          <cell r="C13">
-            <v>7857</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>2</v>
-          </cell>
-          <cell r="C14">
-            <v>7318</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>2</v>
-          </cell>
-          <cell r="C15">
-            <v>7773</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>2</v>
-          </cell>
-          <cell r="C16">
-            <v>7642</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>2</v>
-          </cell>
-          <cell r="C17">
-            <v>7798</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>2</v>
-          </cell>
-          <cell r="C18">
-            <v>6815</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>2</v>
-          </cell>
-          <cell r="C19">
-            <v>6594</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>2</v>
-          </cell>
-          <cell r="C20">
-            <v>6774</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>2</v>
-          </cell>
-          <cell r="C21">
-            <v>7381</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>22 a 27 semanas</v>
-          </cell>
-          <cell r="C22">
-            <v>81008</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>3</v>
-          </cell>
-          <cell r="C23">
-            <v>6732</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>3</v>
-          </cell>
-          <cell r="C24">
-            <v>6409</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>3</v>
-          </cell>
-          <cell r="C25">
-            <v>6591</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>3</v>
-          </cell>
-          <cell r="C26">
-            <v>6079</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>3</v>
-          </cell>
-          <cell r="C27">
-            <v>5929</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>3</v>
-          </cell>
-          <cell r="C28">
-            <v>5868</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>3</v>
-          </cell>
-          <cell r="C29">
-            <v>5398</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>3</v>
-          </cell>
-          <cell r="C30">
-            <v>5057</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>3</v>
-          </cell>
-          <cell r="C31">
-            <v>5043</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>3</v>
-          </cell>
-          <cell r="C32">
-            <v>5075</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>3</v>
-          </cell>
-          <cell r="C33">
-            <v>4824</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>28 a 31 semanas</v>
-          </cell>
-          <cell r="C34">
-            <v>63005</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>4</v>
-          </cell>
-          <cell r="C35">
-            <v>9023</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>4</v>
-          </cell>
-          <cell r="C36">
-            <v>8515</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>4</v>
-          </cell>
-          <cell r="C37">
-            <v>8318</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>4</v>
-          </cell>
-          <cell r="C38">
-            <v>7816</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>4</v>
-          </cell>
-          <cell r="C39">
-            <v>7964</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>4</v>
-          </cell>
-          <cell r="C40">
-            <v>7910</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>4</v>
-          </cell>
-          <cell r="C41">
-            <v>8057</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>4</v>
-          </cell>
-          <cell r="C42">
-            <v>6110</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>4</v>
-          </cell>
-          <cell r="C43">
-            <v>6089</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>4</v>
-          </cell>
-          <cell r="C44">
-            <v>6100</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>4</v>
-          </cell>
-          <cell r="C45">
-            <v>6071</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46" t="str">
-            <v>32 a 36 semanas</v>
-          </cell>
-          <cell r="C46">
-            <v>81973</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>5</v>
-          </cell>
-          <cell r="C47">
-            <v>15122</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>5</v>
-          </cell>
-          <cell r="C48">
-            <v>14612</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>5</v>
-          </cell>
-          <cell r="C49">
-            <v>14211</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>5</v>
-          </cell>
-          <cell r="C50">
-            <v>13685</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>5</v>
-          </cell>
-          <cell r="C51">
-            <v>13938</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52">
-            <v>5</v>
-          </cell>
-          <cell r="C52">
-            <v>13417</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53">
-            <v>5</v>
-          </cell>
-          <cell r="C53">
-            <v>12709</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54">
-            <v>5</v>
-          </cell>
-          <cell r="C54">
-            <v>9674</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="B55">
-            <v>5</v>
-          </cell>
-          <cell r="C55">
-            <v>9232</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="B56">
-            <v>5</v>
-          </cell>
-          <cell r="C56">
-            <v>9489</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="B57">
-            <v>5</v>
-          </cell>
-          <cell r="C57">
-            <v>9486</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="B58" t="str">
-            <v>37 a 41 semanas</v>
-          </cell>
-          <cell r="C58">
-            <v>135575</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="B59">
-            <v>9</v>
-          </cell>
-          <cell r="C59">
-            <v>1351</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="B60">
-            <v>9</v>
-          </cell>
-          <cell r="C60">
-            <v>1214</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="B61">
-            <v>9</v>
-          </cell>
-          <cell r="C61">
-            <v>1293</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="B62" t="str">
-            <v>42 ou mais semanas</v>
-          </cell>
-          <cell r="C62">
-            <v>3858</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11937,8 +11538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C310"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A310" sqref="A310"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="R197" sqref="R197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="2" x14ac:dyDescent="0.35"/>
@@ -15335,7 +14936,8 @@
     <sortCondition ref="B2:B298"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -49096,7 +48698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>

</xml_diff>